<commit_message>
Switch statement for days of the week
</commit_message>
<xml_diff>
--- a/Turni mensa x Paolo.xlsx
+++ b/Turni mensa x Paolo.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SERVERSSN\profili_amministrazione$\valeria.parigi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO M700\PROGRAMMAZIONE IN WINDOWS\C #\PROGETTI PERSONALI IN C#\CalcolaTotaleAlunni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{484A84C4-9221-4561-93A6-AEEF9674EFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="20400" windowHeight="11385" xr2:uid="{B1305039-5561-47D1-A9D6-9A958583801D}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="20400" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="TURNI MENSA CLASSI" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>TURNI CLASSI</t>
   </si>
@@ -207,11 +206,26 @@
       <t>M</t>
     </r>
   </si>
+  <si>
+    <t>0 1</t>
+  </si>
+  <si>
+    <t>2 3</t>
+  </si>
+  <si>
+    <t>4 5</t>
+  </si>
+  <si>
+    <t>6 7</t>
+  </si>
+  <si>
+    <t>8 9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -265,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,39 +428,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -756,14 +782,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB62B962-8216-44DF-8604-C0B31AD06EEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,124 +805,148 @@
     <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:3" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="F3" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6" t="s">
+      <c r="F4" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="F5" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="7" t="s">
+      <c r="F6" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="F7" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7" t="s">
+      <c r="F8" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="F9" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="7" t="s">
+      <c r="F10" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>